<commit_message>
converting data format -> make sure you check NAs
</commit_message>
<xml_diff>
--- a/codebook/Organized Codes.xlsx
+++ b/codebook/Organized Codes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24120" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>95-96</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Race (MONRACE)</t>
   </si>
   <si>
-    <t>Sex (SEX)</t>
-  </si>
-  <si>
     <t>Age (AGE)</t>
   </si>
   <si>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>Sex (MONSEX)</t>
+  </si>
+  <si>
+    <t>Total maximum statuary prison requirement (STAMAX)</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M21"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,392 +433,395 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="25.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="3" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="3"/>
+    <col min="7" max="8" width="25.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" style="3" customWidth="1"/>
+    <col min="13" max="14" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="96" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1"/>
+        <v>16</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1999</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2000</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2001</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2002</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2004</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2005</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2006</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2007</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2008</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2009</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2010</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2011</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2012</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2013</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2014</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="1"/>
+        <v>17</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2015</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
       <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Collapsed education variable down to 5! 0 = No education, 1 = Less than HS, 2 = HS/GED, 3 = Special degree/2 year degrees, 4 = 4 yr college, 5 = graduate degree
</commit_message>
<xml_diff>
--- a/codebook/Organized Codes.xlsx
+++ b/codebook/Organized Codes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
     <t>95-96</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Age (AGE)</t>
   </si>
   <si>
-    <t>Total minimum statuary prison requirement (STAMIN)</t>
-  </si>
-  <si>
     <t>Trial/Plea, etc. (DISPOSIT)</t>
   </si>
   <si>
@@ -71,52 +68,31 @@
     <t>Education (EDUCATN)</t>
   </si>
   <si>
-    <t>Manually added</t>
-  </si>
-  <si>
     <t>Year Sentenced (YEAR)</t>
   </si>
   <si>
-    <t>0 = Male 1 = FEMALE,  9 = Missing or indeterminable</t>
-  </si>
-  <si>
     <t>"</t>
   </si>
   <si>
     <t>Sex (MONSEX)</t>
   </si>
   <si>
-    <t>Total maximum statuary prison requirement (STAMAX)</t>
-  </si>
-  <si>
-    <t> Offender's race (self-reported to the probation officer). Code 8 is not available prior to FY2007. Code 9 is not available prior to FY2009. NOTE: Hispanic ethnicity is coded in the variable HISPORIG. Race and ethnicity are combined in NEWRACE.</t>
-  </si>
-  <si>
-    <t> 1 = White/Caucasian</t>
-  </si>
-  <si>
-    <t>2 = Black/African American</t>
-  </si>
-  <si>
-    <t>3 = American Indian\Alaskan Native</t>
-  </si>
-  <si>
-    <t>4 = Asian or Pacific Islander</t>
-  </si>
-  <si>
-    <t>5 = Multi-racial</t>
-  </si>
-  <si>
-    <t>7 = Other</t>
-  </si>
-  <si>
-    <t>8 = Info on Race Not Available in Docs (This code only available</t>
-  </si>
-  <si>
-    <t>9 = Non-US American Indians (coded to 3 after 2009)</t>
-  </si>
-  <si>
-    <t>NA = Missing, Indeterminable, or inapplicable</t>
+    <t xml:space="preserve">1 = white/caucasian, 2 = black, 3 = american indian, 4, asian/pacific islander, 5  = other (by modification) </t>
+  </si>
+  <si>
+    <t>manually added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = Male 1 = FEMALE,  9 = Missing or indeterminable (by modification) </t>
+  </si>
+  <si>
+    <t>Total minimum statuary prison (STAMIN)</t>
+  </si>
+  <si>
+    <t>Total maximum statuary prison (STAMAX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limit to under 1000 </t>
   </si>
 </sst>
 </file>
@@ -467,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,54 +468,59 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="2"/>
       <c r="M2" s="1"/>
@@ -550,10 +531,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -567,10 +548,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -584,10 +565,10 @@
         <v>1999</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -601,10 +582,10 @@
         <v>2000</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -618,10 +599,10 @@
         <v>2001</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I7" s="1"/>
       <c r="K7" s="1"/>
@@ -634,10 +615,10 @@
         <v>2002</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -651,10 +632,10 @@
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -668,10 +649,10 @@
         <v>2004</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -685,10 +666,10 @@
         <v>2005</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -702,10 +683,10 @@
         <v>2006</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -719,10 +700,10 @@
         <v>2007</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -736,10 +717,10 @@
         <v>2008</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -753,10 +734,10 @@
         <v>2009</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -770,10 +751,10 @@
         <v>2010</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -787,10 +768,10 @@
         <v>2011</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -804,10 +785,10 @@
         <v>2012</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -821,10 +802,10 @@
         <v>2013</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -838,10 +819,10 @@
         <v>2014</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -850,18 +831,16 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2015</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
@@ -873,49 +852,31 @@
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="B29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>

</xml_diff>

<commit_message>
Codebooks, and data visualization!
</commit_message>
<xml_diff>
--- a/codebook/Organized Codes.xlsx
+++ b/codebook/Organized Codes.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="14100" yWindow="480" windowWidth="14700" windowHeight="16720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Race (MONRACE)</t>
   </si>
@@ -87,6 +88,57 @@
   </si>
   <si>
     <t>numeric (manually added)</t>
+  </si>
+  <si>
+    <t>Citizenship (CITIZEN)</t>
+  </si>
+  <si>
+    <t>1 = US Citizen, 2 = "Resident/Legal Alien, 3 = Illegal Alien, 4 = Other</t>
+  </si>
+  <si>
+    <t>Violent Offenses</t>
+  </si>
+  <si>
+    <t>Property offenses</t>
+  </si>
+  <si>
+    <t>Drug offenses</t>
+  </si>
+  <si>
+    <t>Public Order offenses</t>
+  </si>
+  <si>
+    <t>Weapon offenses</t>
+  </si>
+  <si>
+    <t>Immigration offenses</t>
+  </si>
+  <si>
+    <t>95-96</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>9,15,16,17,18,19</t>
+  </si>
+  <si>
+    <t>8,20,21,22,23,24,28, 31,32,33</t>
+  </si>
+  <si>
+    <t>25,26,28,29,30,35</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,36</t>
+  </si>
+  <si>
+    <t>10,11,12,34,37</t>
+  </si>
+  <si>
+    <t>13,14,38</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -467,83 +519,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="7" width="25.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="3" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="3"/>
+    <col min="1" max="2" width="49" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="8" width="25.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" style="3" customWidth="1"/>
+    <col min="13" max="14" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="208" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="208" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
@@ -552,13 +607,13 @@
         <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>17</v>
@@ -569,229 +624,313 @@
       <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="4"/>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C3" s="4"/>
-      <c r="H3" s="1"/>
+      <c r="D3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="4"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C4" s="4"/>
-      <c r="H4" s="1"/>
+      <c r="D4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C5" s="4"/>
-      <c r="H5" s="1"/>
+      <c r="D5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C6" s="4"/>
-      <c r="H6" s="1"/>
+      <c r="D6" s="4"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C7" s="4"/>
-      <c r="H7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="1"/>
+      <c r="D7" s="4"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="4"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C8" s="4"/>
-      <c r="H8" s="1"/>
+      <c r="D8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C9" s="4"/>
-      <c r="H9" s="1"/>
+      <c r="D9" s="4"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="4"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C10" s="4"/>
-      <c r="H10" s="1"/>
+      <c r="D10" s="4"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="4"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C11" s="4"/>
-      <c r="H11" s="1"/>
+      <c r="D11" s="4"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C12" s="4"/>
-      <c r="H12" s="1"/>
+      <c r="D12" s="4"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C13" s="4"/>
-      <c r="H13" s="1"/>
+      <c r="D13" s="4"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="4"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C14" s="4"/>
-      <c r="H14" s="1"/>
+      <c r="D14" s="4"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C15" s="4"/>
-      <c r="H15" s="1"/>
+      <c r="D15" s="4"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C16" s="4"/>
-      <c r="H16" s="1"/>
+      <c r="D16" s="4"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C17" s="4"/>
-      <c r="H17" s="1"/>
+      <c r="D17" s="4"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C18" s="4"/>
-      <c r="H18" s="1"/>
+      <c r="D18" s="4"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="4"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C19" s="4"/>
-      <c r="H19" s="1"/>
+      <c r="D19" s="4"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="4"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C20" s="4"/>
-      <c r="H20" s="1"/>
+      <c r="D20" s="4"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="4"/>
-      <c r="H21" s="1"/>
+      <c r="D21" s="4"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new variable - TYPE - tells us the offense type (with focus in violent, drug, and gun offenses). This commit also includes .gif graphics from gg_animate
</commit_message>
<xml_diff>
--- a/codebook/Organized Codes.xlsx
+++ b/codebook/Organized Codes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14100" yWindow="460" windowWidth="14700" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="14100" yWindow="460" windowWidth="14700" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Race (MONRACE)</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>0 = Male 1 = FEMALE</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>0 = All Others, 1 = Drug Crimes, 2 = firearms, 3 = immigration, 4 = violent crimes</t>
   </si>
 </sst>
 </file>
@@ -522,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +549,7 @@
     <col min="14" max="15" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="80" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -589,8 +595,11 @@
       <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="160" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -636,8 +645,11 @@
       <c r="O2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="J3" s="1"/>
@@ -647,7 +659,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="J4" s="1"/>
@@ -657,7 +669,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="J5" s="1"/>
@@ -667,7 +679,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="J6" s="1"/>
@@ -677,7 +689,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="J7" s="1"/>
@@ -686,7 +698,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="J8" s="1"/>
@@ -696,7 +708,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="J9" s="1"/>
@@ -706,7 +718,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="J10" s="1"/>
@@ -716,7 +728,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="J11" s="1"/>
@@ -726,7 +738,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="J12" s="1"/>
@@ -736,7 +748,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="J13" s="1"/>
@@ -746,7 +758,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="J14" s="1"/>
@@ -756,7 +768,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="J15" s="1"/>
@@ -766,7 +778,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="J16" s="1"/>

</xml_diff>